<commit_message>
Enforced creation of just a single Organisation root object.
</commit_message>
<xml_diff>
--- a/tests/export/fixtures/sample-assets.xlsx
+++ b/tests/export/fixtures/sample-assets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="stations-missing-type" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="60">
   <si>
     <t xml:space="preserve">stations</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t xml:space="preserve">transmission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closest_landmark</t>
   </si>
   <si>
     <t xml:space="preserve">Station1</t>
@@ -207,7 +213,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -230,87 +236,6 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -324,54 +249,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -386,27 +269,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -417,7 +285,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -441,165 +309,41 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -614,7 +358,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>
@@ -773,7 +517,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.19"/>
@@ -931,11 +675,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.19"/>
@@ -943,12 +687,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.66"/>
@@ -984,36 +729,41 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -1029,21 +779,23 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -1059,21 +811,23 @@
         <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AMJ4" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1093,11 +847,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.19"/>
@@ -1105,12 +859,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.66"/>
@@ -1146,96 +901,105 @@
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="3"/>
@@ -1249,10 +1013,10 @@
     </row>
     <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1260,7 +1024,7 @@
     </row>
     <row r="8" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>33000</v>
@@ -1271,10 +1035,10 @@
     </row>
     <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
@@ -1292,16 +1056,16 @@
         <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AMB9" s="0"/>
       <c r="AMC9" s="0"/>
@@ -1318,16 +1082,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
@@ -1339,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AMB10" s="0"/>
       <c r="AMC10" s="0"/>
@@ -1356,16 +1120,16 @@
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>22</v>
@@ -1377,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AMB11" s="0"/>
       <c r="AMC11" s="0"/>

</xml_diff>